<commit_message>
correct status detail sbp, dbp, heart rate and phy commuting
</commit_message>
<xml_diff>
--- a/data_processing_elements-NES.xlsx
+++ b/data_processing_elements-NES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5441A05E-3EB2-41BE-A5F9-C050EB309865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D886E7A1-8659-4296-849C-AC372801F8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -3391,10 +3391,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J82" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T91" sqref="T91"/>
+      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4725,7 +4725,7 @@
         <v>27</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="R25" s="1" t="s">
         <v>208</v>
@@ -4782,7 +4782,7 @@
         <v>27</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="R26" s="1" t="s">
         <v>208</v>
@@ -4839,7 +4839,7 @@
         <v>27</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>208</v>
@@ -7616,7 +7616,7 @@
         <v>27</v>
       </c>
       <c r="Q81" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="R81" s="1" t="s">
         <v>208</v>

</xml_diff>